<commit_message>
enabled 3 E2E tests for McPizza Bot
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C4A40D-B040-45E4-B4B3-7E4A0BA74098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E3C6FD-0509-4EAC-B94C-B52960B2BCE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
   <si>
     <t>testname</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>I want to order a pizza</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
   <si>
     <t>query2</t>
@@ -215,12 +212,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -230,21 +242,21 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -586,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -617,36 +629,36 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.5">
-      <c r="A2" s="4" t="s">
-        <v>25</v>
+      <c r="A2" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.5">
-      <c r="A3" s="4" t="s">
-        <v>40</v>
+      <c r="A3" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -660,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -704,142 +716,151 @@
         <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="28.5">
-      <c r="A2" s="4" t="s">
-        <v>25</v>
+      <c r="A2" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="H2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="28.5">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="L3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15" ht="28.5">
-      <c r="A4" s="4" t="s">
-        <v>40</v>
+      <c r="A4" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>43</v>
+      <c r="G4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="9" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
segregatted placeOrder and submitFeeddback test scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E3C6FD-0509-4EAC-B94C-B52960B2BCE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6D5597-F93F-40FF-9CED-F6B75F1B9BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
   <si>
     <t>testname</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>I am sorry I dont have an answer for that</t>
+  </si>
+  <si>
+    <t>giveFeedbackOrderMcPizza</t>
+  </si>
+  <si>
+    <t>Submit Feedback to McPIizza bot</t>
+  </si>
+  <si>
+    <t>Feedback Test</t>
   </si>
 </sst>
 </file>
@@ -596,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -662,6 +671,23 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:5" ht="28.5">
+      <c r="A4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -670,10 +696,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -780,9 +806,7 @@
       <c r="M2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="N2" s="7"/>
       <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="28.5">
@@ -825,9 +849,7 @@
       <c r="M3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="N3" s="7"/>
       <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15" ht="28.5">
@@ -863,13 +885,59 @@
         <v>42</v>
       </c>
     </row>
+    <row r="5" spans="1:15" ht="28.5">
+      <c r="A5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="4"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{633031F1-9F49-4A83-9747-38EF42C7FA15}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{9F3ACF45-85CE-4735-BDBE-1E2353A29837}"/>
     <hyperlink ref="F4" r:id="rId3" xr:uid="{8799B1D0-AA5B-432C-BB68-1D8EE935E59F}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{8A5FA54C-1E89-44E1-BD4A-007D6B3ED455}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>